<commit_message>
Add currency setting and minimum start row
</commit_message>
<xml_diff>
--- a/stockx_book.xlsx
+++ b/stockx_book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohhanyi/Documents/backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohhanyi/stockx-inventory-updater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C208ACCA-D337-BB4F-8C71-FBD5321A9432}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41F5C58-DB4D-5645-98D8-9DF48915625B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="4060" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -90,10 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -416,17 +412,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,25 +445,6 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add error handling and change default book
</commit_message>
<xml_diff>
--- a/stockx_book.xlsx
+++ b/stockx_book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohhanyi/stockx-inventory-updater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41F5C58-DB4D-5645-98D8-9DF48915625B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A893BE-BA76-C741-A4F8-359B1A2D9E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="4060" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Style Code</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>Last Updated</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Sold</t>
+  </si>
+  <si>
+    <t>Price Sold</t>
   </si>
 </sst>
 </file>
@@ -87,14 +96,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -105,6 +143,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K115" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:K115" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K109">
+    <sortCondition ref="B2:B109"/>
+    <sortCondition ref="C2:C109"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Style Code"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Product Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Size" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Selling Price"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Stockx Last Sale"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Stockx Average (last 3 sales)"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Stockx Link"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Last Updated"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Location"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Sold"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Price Sold"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,49 +466,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add highest bid and lowest ask
</commit_message>
<xml_diff>
--- a/stockx_book.xlsx
+++ b/stockx_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohhanyi/stockx-inventory-updater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A893BE-BA76-C741-A4F8-359B1A2D9E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9180A2-EFE2-2740-B11F-98769338C3D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Style Code</t>
   </si>
@@ -53,13 +53,19 @@
   </si>
   <si>
     <t>Price Sold</t>
+  </si>
+  <si>
+    <t>Highest Bid</t>
+  </si>
+  <si>
+    <t>Lowest Ask</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,6 +77,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,19 +158,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K115" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:K115" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M115" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:M115" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M109">
     <sortCondition ref="B2:B109"/>
     <sortCondition ref="C2:C109"/>
   </sortState>
-  <tableColumns count="11">
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Style Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Product Name"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Size" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Selling Price"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Stockx Last Sale"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Stockx Average (last 3 sales)"/>
+    <tableColumn id="12" xr3:uid="{FA7DE45B-E918-9341-9C0A-86EA97E18A9E}" name="Highest Bid"/>
+    <tableColumn id="13" xr3:uid="{EAF8FF8C-709F-7F4F-8160-E8773B29D1A1}" name="Lowest Ask"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Stockx Link"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Last Updated"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Location"/>
@@ -466,11 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,12 +495,14 @@
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -506,22 +522,29 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>